<commit_message>
Bus movements and streetcar shuttle garage changes
</commit_message>
<xml_diff>
--- a/Bus Allocations.xlsx
+++ b/Bus Allocations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lawre\OneDrive\Desktop\TTC_RAD_tracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lawre\OneDrive\Desktop\TTC-RAD-Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF03DD9-5410-4916-84F0-7CBD57F3B09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FA16E1-356B-4E3B-94D6-E5E620CB0BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5106EA48-F6EC-48B3-9B00-4A377D782005}"/>
   </bookViews>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E4B37F-218A-4E51-8601-1E570BBEE6AD}">
   <dimension ref="A1:CAA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="ZQ1" workbookViewId="0">
-      <selection activeCell="AAC3" sqref="AAC3"/>
+    <sheetView tabSelected="1" topLeftCell="BZD1" workbookViewId="0">
+      <selection activeCell="BZV2" sqref="BZV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8716,19 +8716,19 @@
         <v>1</v>
       </c>
       <c r="AAI2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AAJ2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AAK2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AAL2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AAM2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AAN2" t="s">
         <v>4</v>
@@ -12406,10 +12406,10 @@
         <v>1</v>
       </c>
       <c r="BVQ2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BVR2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BVS2" t="s">
         <v>0</v>
@@ -12706,34 +12706,34 @@
         <v>5</v>
       </c>
       <c r="BZM2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BZN2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BZO2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BZP2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BZQ2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BZR2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BZS2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BZT2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BZU2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BZV2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BZW2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Edit readme with 2022-09-07 changes to bus and route allocations
</commit_message>
<xml_diff>
--- a/Bus Allocations.xlsx
+++ b/Bus Allocations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lawre\OneDrive\Desktop\TTC-RAD-Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FA16E1-356B-4E3B-94D6-E5E620CB0BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF347FBF-5876-4C4A-93C6-29733F98E394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5106EA48-F6EC-48B3-9B00-4A377D782005}"/>
   </bookViews>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E4B37F-218A-4E51-8601-1E570BBEE6AD}">
   <dimension ref="A1:CAA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BZD1" workbookViewId="0">
-      <selection activeCell="BZV2" sqref="BZV2"/>
+    <sheetView tabSelected="1" topLeftCell="BXI1" workbookViewId="0">
+      <selection activeCell="BXZ3" sqref="BXZ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12589,7 +12589,7 @@
         <v>4</v>
       </c>
       <c r="BXZ2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BYA2" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
9220 - 9224: BIR -> ARW
</commit_message>
<xml_diff>
--- a/Bus Allocations.xlsx
+++ b/Bus Allocations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lawre\OneDrive\Desktop\TTC-RAD-Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF347FBF-5876-4C4A-93C6-29733F98E394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAA81B9-9904-4B55-9BC9-A86BB1D4E336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5106EA48-F6EC-48B3-9B00-4A377D782005}"/>
   </bookViews>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E4B37F-218A-4E51-8601-1E570BBEE6AD}">
   <dimension ref="A1:CAA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BXI1" workbookViewId="0">
-      <selection activeCell="BXZ3" sqref="BXZ3"/>
+    <sheetView tabSelected="1" topLeftCell="BYS1" workbookViewId="0">
+      <selection activeCell="BZL7" sqref="BZL7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12691,19 +12691,19 @@
         <v>5</v>
       </c>
       <c r="BZH2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BZI2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BZJ2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BZK2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BZL2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BZM2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Added comments and message printed when no special sightings found
</commit_message>
<xml_diff>
--- a/Bus Allocations.xlsx
+++ b/Bus Allocations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lawre\OneDrive\Desktop\TTC-RAD-Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAA81B9-9904-4B55-9BC9-A86BB1D4E336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3B78F4-DBD3-450A-9043-FDA6961FED38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5106EA48-F6EC-48B3-9B00-4A377D782005}"/>
   </bookViews>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E4B37F-218A-4E51-8601-1E570BBEE6AD}">
   <dimension ref="A1:CAA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BYS1" workbookViewId="0">
-      <selection activeCell="BZL7" sqref="BZL7"/>
+    <sheetView tabSelected="1" topLeftCell="BRS1" workbookViewId="0">
+      <selection activeCell="BSF14" sqref="BSF14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11911,16 +11911,16 @@
         <v>6</v>
       </c>
       <c r="BPH2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BPI2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BPJ2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BPK2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BPL2" t="s">
         <v>4</v>
@@ -12127,7 +12127,7 @@
         <v>4</v>
       </c>
       <c r="BSB2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="BSC2" t="s">
         <v>4</v>
@@ -12139,10 +12139,10 @@
         <v>4</v>
       </c>
       <c r="BSF2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="BSG2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="BSH2" t="s">
         <v>4</v>
@@ -12154,25 +12154,25 @@
         <v>4</v>
       </c>
       <c r="BSK2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="BSL2" t="s">
         <v>4</v>
       </c>
       <c r="BSM2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="BSN2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="BSO2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="BSP2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="BSQ2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="BSR2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Arrow received some 31XX
</commit_message>
<xml_diff>
--- a/Bus Allocations.xlsx
+++ b/Bus Allocations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lawre\OneDrive\Desktop\TTC-RAD-Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3B78F4-DBD3-450A-9043-FDA6961FED38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CB5034-BA8D-4E7D-ADFD-8E78BF877E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5106EA48-F6EC-48B3-9B00-4A377D782005}"/>
   </bookViews>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E4B37F-218A-4E51-8601-1E570BBEE6AD}">
   <dimension ref="A1:CAA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BRS1" workbookViewId="0">
-      <selection activeCell="BSF14" sqref="BSF14"/>
+    <sheetView tabSelected="1" topLeftCell="MO1" workbookViewId="0">
+      <selection activeCell="MY6" sqref="MY6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7654,7 +7654,7 @@
         <v>2</v>
       </c>
       <c r="MS2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="MT2" t="s">
         <v>2</v>
@@ -7666,13 +7666,13 @@
         <v>2</v>
       </c>
       <c r="MW2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="MX2" t="s">
         <v>2</v>
       </c>
       <c r="MY2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="MZ2" t="s">
         <v>2</v>
@@ -7684,7 +7684,7 @@
         <v>2</v>
       </c>
       <c r="NC2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="ND2" t="s">
         <v>2</v>
@@ -7696,7 +7696,7 @@
         <v>2</v>
       </c>
       <c r="NG2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="NH2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
1392-> WIL; 3322, 3326->QSY
</commit_message>
<xml_diff>
--- a/Bus Allocations.xlsx
+++ b/Bus Allocations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lawre\OneDrive\Desktop\TTC-RAD-Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785CA3D6-DB8B-468B-8A35-76A50CD11F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C722C5-A4DA-4D77-A434-341B74945FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5106EA48-F6EC-48B3-9B00-4A377D782005}"/>
   </bookViews>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E4B37F-218A-4E51-8601-1E570BBEE6AD}">
   <dimension ref="A1:CAA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="JO1" workbookViewId="0">
-      <selection activeCell="JZ3" sqref="JZ3"/>
+    <sheetView tabSelected="1" topLeftCell="UU1" workbookViewId="0">
+      <selection activeCell="VB3" sqref="VB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7438,7 +7438,7 @@
         <v>7</v>
       </c>
       <c r="JY2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="JZ2" t="s">
         <v>7</v>
@@ -8305,7 +8305,7 @@
         <v>3</v>
       </c>
       <c r="VB2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="VC2" t="s">
         <v>3</v>
@@ -8317,7 +8317,7 @@
         <v>3</v>
       </c>
       <c r="VF2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="VG2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
3100, 3122, 3125 -> McN
</commit_message>
<xml_diff>
--- a/Bus Allocations.xlsx
+++ b/Bus Allocations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lawre\OneDrive\Desktop\TTC-RAD-Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C722C5-A4DA-4D77-A434-341B74945FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63591581-F033-43A9-A651-6B70696505EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5106EA48-F6EC-48B3-9B00-4A377D782005}"/>
   </bookViews>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E4B37F-218A-4E51-8601-1E570BBEE6AD}">
   <dimension ref="A1:CAA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="UU1" workbookViewId="0">
-      <selection activeCell="VB3" sqref="VB3"/>
+    <sheetView tabSelected="1" topLeftCell="MR1" workbookViewId="0">
+      <selection activeCell="MZ17" sqref="MZ17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7639,7 +7639,7 @@
         <v>1</v>
       </c>
       <c r="MN2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="MO2" t="s">
         <v>2</v>
@@ -7705,7 +7705,7 @@
         <v>2</v>
       </c>
       <c r="NJ2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="NK2" t="s">
         <v>2</v>
@@ -7714,7 +7714,7 @@
         <v>2</v>
       </c>
       <c r="NM2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="NN2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
movements and 301/501 added to MTD
</commit_message>
<xml_diff>
--- a/Bus Allocations.xlsx
+++ b/Bus Allocations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lawre\OneDrive\Desktop\TTC-RAD-Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972D9030-8B9A-400C-B55F-0A3DD57132E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58602FE-0ADC-4D82-A778-8E10678AA3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13668" yWindow="2664" windowWidth="7500" windowHeight="9276" xr2:uid="{5106EA48-F6EC-48B3-9B00-4A377D782005}"/>
   </bookViews>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E4B37F-218A-4E51-8601-1E570BBEE6AD}">
   <dimension ref="A1:CAA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="UT1" workbookViewId="0">
-      <selection activeCell="UX2" sqref="UX2"/>
+    <sheetView tabSelected="1" topLeftCell="UW1" workbookViewId="0">
+      <selection activeCell="VB6" sqref="VB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8269,28 +8269,28 @@
         <v>3</v>
       </c>
       <c r="UP2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="UQ2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="UR2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="US2" t="s">
         <v>3</v>
       </c>
       <c r="UT2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="UU2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="UV2" t="s">
         <v>3</v>
       </c>
       <c r="UW2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="UX2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Major update. Now shows runs, next departures, and eliminates school specials.
</commit_message>
<xml_diff>
--- a/Bus Allocations.xlsx
+++ b/Bus Allocations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lawre\OneDrive\Desktop\TTC-RAD-Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58602FE-0ADC-4D82-A778-8E10678AA3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6D9D12-6BBA-4435-838E-C392DCB5C884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13668" yWindow="2664" windowWidth="7500" windowHeight="9276" xr2:uid="{5106EA48-F6EC-48B3-9B00-4A377D782005}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5106EA48-F6EC-48B3-9B00-4A377D782005}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E4B37F-218A-4E51-8601-1E570BBEE6AD}">
   <dimension ref="A1:CAA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="UW1" workbookViewId="0">
-      <selection activeCell="VB6" sqref="VB6"/>
+    <sheetView tabSelected="1" topLeftCell="IR1" workbookViewId="0">
+      <selection activeCell="JC3" sqref="JC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7372,7 +7372,7 @@
         <v>7</v>
       </c>
       <c r="JC2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="JD2" t="s">
         <v>7</v>

</xml_diff>